<commit_message>
Report at 4000 words and Gantt Chart revised
</commit_message>
<xml_diff>
--- a/documents/Project_GanttChart.xlsx
+++ b/documents/Project_GanttChart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\College\4th year\FYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\College\4th year\FYP\The_Truth_about_Twitter\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5EC1A874-AA94-4BCB-8BD4-E2DAD6D85FE4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56E9526E-C643-495B-91DE-18022299F450}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{DC48C0EB-4A74-456B-A167-C1FE483EEF7C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
   <si>
     <t>Stage Name</t>
   </si>
@@ -97,6 +97,21 @@
   </si>
   <si>
     <t>Data UnderStanding &amp; Prep</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -401,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -477,6 +492,15 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -492,15 +516,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,16 +608,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -616,7 +632,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5124450" y="9525"/>
+          <a:off x="5372100" y="57150"/>
           <a:ext cx="1" cy="3429000"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1061,7 +1077,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,54 +1088,54 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="62" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="55" t="s">
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="56" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="56"/>
-      <c r="T1" s="56"/>
-      <c r="U1" s="56"/>
-      <c r="V1" s="57" t="s">
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="57"/>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="58" t="s">
+      <c r="W1" s="60"/>
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="59" t="s">
+      <c r="AA1" s="61"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
-      <c r="AG1" s="59"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
     </row>
     <row r="2" spans="1:33" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -1279,8 +1295,12 @@
       <c r="O4" s="49"/>
       <c r="P4" s="12"/>
       <c r="Q4" s="13"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="47"/>
+      <c r="R4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="63" t="s">
+        <v>24</v>
+      </c>
       <c r="T4" s="48"/>
       <c r="U4" s="48"/>
       <c r="V4" s="48"/>
@@ -1316,8 +1336,12 @@
       <c r="O5" s="13"/>
       <c r="P5" s="12"/>
       <c r="Q5" s="13"/>
-      <c r="R5" s="27"/>
-      <c r="S5" s="29"/>
+      <c r="R5" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>25</v>
+      </c>
       <c r="T5" s="27"/>
       <c r="U5" s="29"/>
       <c r="V5" s="32"/>
@@ -1353,8 +1377,12 @@
       <c r="O6" s="13"/>
       <c r="P6" s="12"/>
       <c r="Q6" s="13"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="29"/>
+      <c r="R6" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" s="29" t="s">
+        <v>26</v>
+      </c>
       <c r="T6" s="27"/>
       <c r="U6" s="29"/>
       <c r="V6" s="32"/>
@@ -1390,8 +1418,12 @@
       <c r="O7" s="13"/>
       <c r="P7" s="12"/>
       <c r="Q7" s="13"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="29"/>
+      <c r="R7" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="S7" s="29" t="s">
+        <v>27</v>
+      </c>
       <c r="T7" s="27"/>
       <c r="U7" s="29"/>
       <c r="V7" s="32"/>
@@ -1425,10 +1457,14 @@
       <c r="M8" s="48"/>
       <c r="N8" s="49"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="29"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="S8" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="T8" s="27"/>
       <c r="U8" s="29"/>
       <c r="V8" s="32"/>
@@ -1458,8 +1494,8 @@
       <c r="I9" s="7"/>
       <c r="J9" s="6"/>
       <c r="K9" s="7"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="50"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="49"/>
       <c r="N9" s="12"/>
       <c r="O9" s="13"/>
       <c r="P9" s="12"/>
@@ -1495,8 +1531,8 @@
       <c r="I10" s="7"/>
       <c r="J10" s="47"/>
       <c r="K10" s="48"/>
-      <c r="L10" s="49"/>
-      <c r="M10" s="13"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="49"/>
       <c r="N10" s="12"/>
       <c r="O10" s="13"/>
       <c r="P10" s="12"/>
@@ -1668,7 +1704,8 @@
       <c r="E15" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="46" t="s">
+      <c r="L15" s="46"/>
+      <c r="M15" s="46" t="s">
         <v>19</v>
       </c>
       <c r="N15" s="46" t="s">
@@ -1680,14 +1717,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:L1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Table of contents and figures updated and report formatting
</commit_message>
<xml_diff>
--- a/documents/Project_GanttChart.xlsx
+++ b/documents/Project_GanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\College\4th year\FYP\The_Truth_about_Twitter\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56E9526E-C643-495B-91DE-18022299F450}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{319D7E00-1D1D-4C78-AF12-CCBA4A531130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" xr2:uid="{DC48C0EB-4A74-456B-A167-C1FE483EEF7C}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>VP</t>
   </si>
   <si>
-    <t>Build Basic Client App</t>
-  </si>
-  <si>
     <t>Data UnderStanding &amp; Prep</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Build Web Front End</t>
   </si>
 </sst>
 </file>
@@ -492,6 +492,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -507,16 +517,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,54 +1088,54 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="C1" s="59"/>
+      <c r="D1" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="57" t="s">
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="s">
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="59" t="s">
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="59"/>
-      <c r="T1" s="59"/>
-      <c r="U1" s="59"/>
-      <c r="V1" s="60" t="s">
+      <c r="S1" s="63"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="60"/>
-      <c r="X1" s="60"/>
-      <c r="Y1" s="60"/>
-      <c r="Z1" s="61" t="s">
+      <c r="W1" s="56"/>
+      <c r="X1" s="56"/>
+      <c r="Y1" s="56"/>
+      <c r="Z1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="AA1" s="61"/>
-      <c r="AB1" s="61"/>
-      <c r="AC1" s="61"/>
-      <c r="AD1" s="62" t="s">
+      <c r="AA1" s="57"/>
+      <c r="AB1" s="57"/>
+      <c r="AC1" s="57"/>
+      <c r="AD1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
+      <c r="AG1" s="58"/>
     </row>
     <row r="2" spans="1:33" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="25" t="s">
@@ -1296,10 +1296,10 @@
       <c r="P4" s="12"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="63" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="S4" s="55" t="s">
+        <v>23</v>
       </c>
       <c r="T4" s="48"/>
       <c r="U4" s="48"/>
@@ -1337,10 +1337,10 @@
       <c r="P5" s="12"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S5" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T5" s="27"/>
       <c r="U5" s="29"/>
@@ -1378,10 +1378,10 @@
       <c r="P6" s="12"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S6" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T6" s="27"/>
       <c r="U6" s="29"/>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
@@ -1419,10 +1419,10 @@
       <c r="P7" s="12"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S7" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="T7" s="27"/>
       <c r="U7" s="29"/>
@@ -1460,10 +1460,10 @@
       <c r="P8" s="47"/>
       <c r="Q8" s="49"/>
       <c r="R8" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S8" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T8" s="27"/>
       <c r="U8" s="29"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="2"/>
@@ -1502,10 +1502,10 @@
       <c r="Q9" s="13"/>
       <c r="R9" s="27"/>
       <c r="S9" s="29"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="29"/>
-      <c r="V9" s="32"/>
-      <c r="W9" s="34"/>
+      <c r="T9" s="47"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="49"/>
       <c r="X9" s="32"/>
       <c r="Y9" s="34"/>
       <c r="Z9" s="37"/>

</xml_diff>